<commit_message>
Ajustes con Tablas e histogramas
</commit_message>
<xml_diff>
--- a/tabla_frecuencias.xlsx
+++ b/tabla_frecuencias.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Clase</t>
   </si>
@@ -34,31 +34,22 @@
     <t>Hi</t>
   </si>
   <si>
-    <t>[46, 52)</t>
-  </si>
-  <si>
-    <t>[52, 58)</t>
-  </si>
-  <si>
-    <t>[58, 64)</t>
-  </si>
-  <si>
-    <t>[64, 70)</t>
-  </si>
-  <si>
-    <t>[70, 76)</t>
-  </si>
-  <si>
-    <t>[76, 82)</t>
-  </si>
-  <si>
-    <t>[82, 88)</t>
-  </si>
-  <si>
-    <t>[88, 94)</t>
-  </si>
-  <si>
-    <t>[94, 100)</t>
+    <t>[54, 61)</t>
+  </si>
+  <si>
+    <t>[61, 68)</t>
+  </si>
+  <si>
+    <t>[68, 75)</t>
+  </si>
+  <si>
+    <t>[75, 82)</t>
+  </si>
+  <si>
+    <t>[82, 89)</t>
+  </si>
+  <si>
+    <t>[89, 96)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -442,19 +433,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>49</v>
+        <v>57.5</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>0.014</v>
+        <v>0.133</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1">
-        <v>0.014</v>
+        <v>0.133</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -462,19 +453,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>55</v>
+        <v>64.5</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>0.07099999999999999</v>
+        <v>0.167</v>
       </c>
       <c r="E3" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
-        <v>0.08599999999999999</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -482,19 +473,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>61</v>
+        <v>71.5</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>0.07099999999999999</v>
+        <v>0.067</v>
       </c>
       <c r="E4" s="1">
         <v>11</v>
       </c>
       <c r="F4" s="1">
-        <v>0.157</v>
+        <v>0.367</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -502,19 +493,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>67</v>
+        <v>78.5</v>
       </c>
       <c r="C5" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
-        <v>0.1</v>
+        <v>0.267</v>
       </c>
       <c r="E5" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1">
-        <v>0.257</v>
+        <v>0.633</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -522,19 +513,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>73</v>
+        <v>85.5</v>
       </c>
       <c r="C6" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
-        <v>0.143</v>
+        <v>0.267</v>
       </c>
       <c r="E6" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -542,78 +533,18 @@
         <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>79</v>
+        <v>92.5</v>
       </c>
       <c r="C7" s="1">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>0.257</v>
+        <v>0.067</v>
       </c>
       <c r="E7" s="1">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1">
-        <v>0.657</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
-        <v>85</v>
-      </c>
-      <c r="C8" s="1">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.157</v>
-      </c>
-      <c r="E8" s="1">
-        <v>57</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.8139999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1">
-        <v>91</v>
-      </c>
-      <c r="C9" s="1">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.114</v>
-      </c>
-      <c r="E9" s="1">
-        <v>65</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.929</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1">
-        <v>97</v>
-      </c>
-      <c r="C10" s="1">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.07099999999999999</v>
-      </c>
-      <c r="E10" s="1">
-        <v>70</v>
-      </c>
-      <c r="F10" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>